<commit_message>
feat(translation): update translation for all languages
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/as/b.xlsx
+++ b/utils/localisation_script/excel_to_json/as/b.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/as/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E513FD93-1D5B-AF4F-96F8-B8CC6A8B4A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30291371-7B57-0E4D-B88E-427E60F3D793}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>Button Label</t>
   </si>
@@ -368,7 +368,7 @@
   <dimension ref="A2:Z901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -384,9 +384,7 @@
   <sheetData>
     <row r="2" spans="1:26" ht="14" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>